<commit_message>
Updated VS Automation: iframe removed for some tabs(fav, lookbook) in microsite
</commit_message>
<xml_diff>
--- a/KatalonProjects/envtData.xlsx
+++ b/KatalonProjects/envtData.xlsx
@@ -65,19 +65,19 @@
     <t>https://mirandakate.cabionline.com/</t>
   </si>
   <si>
-    <t>https://test21.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test21.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test21.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>virtual_cabitest21</t>
-  </si>
-  <si>
-    <t>test21</t>
+    <t>https://test18.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test18.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test18.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>virtual_cabitest18</t>
+  </si>
+  <si>
+    <t>test18</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DTY order status validated Negative Scenario covered
</commit_message>
<xml_diff>
--- a/KatalonProjects/envtData.xlsx
+++ b/KatalonProjects/envtData.xlsx
@@ -65,6 +65,12 @@
     <t>https://mirandakate.cabionline.com/</t>
   </si>
   <si>
+    <t>WMURL</t>
+  </si>
+  <si>
+    <t>http://webmail.cabiclio.com/</t>
+  </si>
+  <si>
     <t>https://test18.cliotest.com/backoffice/control/main</t>
   </si>
   <si>
@@ -78,12 +84,6 @@
   </si>
   <si>
     <t>test18</t>
-  </si>
-  <si>
-    <t>WMURL</t>
-  </si>
-  <si>
-    <t>http://webmail.cabiclio.com/</t>
   </si>
 </sst>
 </file>
@@ -438,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,30 +484,30 @@
         <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -516,7 +516,7 @@
         <v>12</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DTY: Shipping DTY eligible order from workhouse
</commit_message>
<xml_diff>
--- a/KatalonProjects/envtData.xlsx
+++ b/KatalonProjects/envtData.xlsx
@@ -71,19 +71,19 @@
     <t>http://webmail.cabiclio.com/</t>
   </si>
   <si>
-    <t>https://test21.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test21.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test21.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>virtual_cabitest21</t>
-  </si>
-  <si>
-    <t>test21</t>
+    <t>https://test17.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test17.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test17.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>virtual_cabitest17</t>
+  </si>
+  <si>
+    <t>test17</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +521,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://test17.cliotest.com/cabicentral/control/main"/>
+    <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2" display="https://sandbox.cabiclio.com/warehouse/control/main"/>
     <hyperlink ref="E2" r:id="rId3"/>
     <hyperlink ref="A2" r:id="rId4" display="https://test18.cliotest.com/backoffice/control/main"/>

</xml_diff>

<commit_message>
microsite tabs locators updated: vs automation
</commit_message>
<xml_diff>
--- a/KatalonProjects/envtData.xlsx
+++ b/KatalonProjects/envtData.xlsx
@@ -71,19 +71,19 @@
     <t>http://webmail.cabiclio.com/</t>
   </si>
   <si>
-    <t>https://test17.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test17.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test17.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>virtual_cabitest17</t>
-  </si>
-  <si>
-    <t>test17</t>
+    <t>https://test18.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test18.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test18.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>virtual_cabitest18</t>
+  </si>
+  <si>
+    <t>test18</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,10 +521,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://test17.cliotest.com/cabicentral/control/main"/>
     <hyperlink ref="D2" r:id="rId2" display="https://sandbox.cabiclio.com/warehouse/control/main"/>
     <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4" display="https://test18.cliotest.com/backoffice/control/main"/>
+    <hyperlink ref="A2" r:id="rId4"/>
     <hyperlink ref="J2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Order Creation: Show order and Add On Order
</commit_message>
<xml_diff>
--- a/KatalonProjects/envtData.xlsx
+++ b/KatalonProjects/envtData.xlsx
@@ -71,22 +71,22 @@
     <t>http://webmail.cabiclio.com/</t>
   </si>
   <si>
-    <t>https://test18.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test18.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test18.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>virtual_cabitest18</t>
-  </si>
-  <si>
-    <t>test18</t>
-  </si>
-  <si>
     <t>WMEnvt</t>
+  </si>
+  <si>
+    <t>https://test14.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test14.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test14.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>virtual_cabitest14</t>
+  </si>
+  <si>
+    <t>test14</t>
   </si>
 </sst>
 </file>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,30 +490,30 @@
         <v>13</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -525,7 +525,7 @@
         <v>14</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -533,7 +533,7 @@
     <hyperlink ref="C2" r:id="rId1" display="https://test17.cliotest.com/cabicentral/control/main"/>
     <hyperlink ref="D2" r:id="rId2" display="https://sandbox.cabiclio.com/warehouse/control/main"/>
     <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId4" display="https://test18.cliotest.com/backoffice/control/main"/>
     <hyperlink ref="J2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rsEditOrderRS: webui.clicks are replaced by JS executor of webui
</commit_message>
<xml_diff>
--- a/KatalonProjects/envtData.xlsx
+++ b/KatalonProjects/envtData.xlsx
@@ -74,19 +74,19 @@
     <t>WMEnvt</t>
   </si>
   <si>
-    <t>https://test21.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test21.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test21.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>virtual_cabitest21</t>
-  </si>
-  <si>
-    <t>test21</t>
+    <t>https://test18.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test18.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test18.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>virtual_cabitest18</t>
+  </si>
+  <si>
+    <t>test18</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
NA scripts and DataFiles updated in consideration of SR Spring 2020: 1. productVerify updated with new product sizes 2. data files: productData, timeZoneDate updated
</commit_message>
<xml_diff>
--- a/KatalonProjects/envtData.xlsx
+++ b/KatalonProjects/envtData.xlsx
@@ -74,19 +74,19 @@
     <t>WMEnvt</t>
   </si>
   <si>
-    <t>https://test18.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test18.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test18.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>virtual_cabitest18</t>
-  </si>
-  <si>
-    <t>test18</t>
+    <t>https://test7.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test7.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test7.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>virtual_cabitest7</t>
+  </si>
+  <si>
+    <t>test7</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
DTY Edit order parallel
</commit_message>
<xml_diff>
--- a/KatalonProjects/envtData.xlsx
+++ b/KatalonProjects/envtData.xlsx
@@ -74,19 +74,19 @@
     <t>WMEnvt</t>
   </si>
   <si>
-    <t>https://test18.cliotest.com/backoffice/control/main</t>
-  </si>
-  <si>
-    <t>https://test18.cliotest.com/cabicentral/control/main</t>
-  </si>
-  <si>
-    <t>https://test18.cliotest.com/warehouse/control/main</t>
-  </si>
-  <si>
-    <t>virtual_cabitest18</t>
-  </si>
-  <si>
-    <t>test18</t>
+    <t>https://test21.cliotest.com/backoffice/control/main</t>
+  </si>
+  <si>
+    <t>https://test21.cliotest.com/cabicentral/control/main</t>
+  </si>
+  <si>
+    <t>https://test21.cliotest.com/warehouse/control/main</t>
+  </si>
+  <si>
+    <t>virtual_cabitest21</t>
+  </si>
+  <si>
+    <t>test21</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>